<commit_message>
Oculta aba inicio e cria planilha OLD
</commit_message>
<xml_diff>
--- a/Escala.outubro.xlsx
+++ b/Escala.outubro.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8265" windowWidth="18735" xWindow="360" yWindow="300"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8265" windowWidth="18735" xWindow="360" yWindow="300"/>
   </bookViews>
   <sheets>
-    <sheet name="Inicio" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Inicio" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Vermelha" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Preta" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Marrom" sheetId="4" state="visible" r:id="rId4"/>
@@ -21,8 +21,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
-    <numFmt formatCode="dd/mm/yyyy" numFmtId="165"/>
+    <numFmt formatCode="dd/mm/yyyy" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -341,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -451,7 +451,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="22" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="22" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="23" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -470,6 +470,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="22" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -770,10 +771,10 @@
   <dimension ref="A1:CG51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="26.28515625"/>
     <col customWidth="1" max="2" min="2" style="4" width="10.7109375"/>
@@ -1561,7 +1562,9 @@
           <t>2S SAD JULIA</t>
         </is>
       </c>
-      <c r="B29" s="15" t="n"/>
+      <c r="B29" s="15" t="n">
+        <v>43764</v>
+      </c>
       <c r="C29" s="15" t="n"/>
       <c r="D29" s="15" t="n"/>
       <c r="E29" s="15" t="n"/>
@@ -2162,7 +2165,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="22" width="24.5703125"/>
     <col customWidth="1" max="29" min="2" style="1" width="10.7109375"/>
@@ -2176,271 +2179,271 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="inlineStr">
+      <c r="A2" s="58" t="inlineStr">
         <is>
           <t>1S SGS ANDERSON</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="inlineStr">
+      <c r="A3" s="58" t="inlineStr">
         <is>
           <t>1S SAD CLAUDINO</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="inlineStr">
+      <c r="A4" s="58" t="inlineStr">
         <is>
           <t>2S SIN DAVID</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="inlineStr">
+      <c r="A5" s="58" t="inlineStr">
         <is>
           <t>2S SIN VICTOR</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="inlineStr">
+      <c r="A6" s="58" t="inlineStr">
         <is>
           <t>2S SIN SUELEN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="inlineStr">
+      <c r="A7" s="58" t="inlineStr">
         <is>
           <t>2S SCF GISELI</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="inlineStr">
+      <c r="A8" s="58" t="inlineStr">
         <is>
           <t>2S SIN BRUNO</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="inlineStr">
+      <c r="A9" s="58" t="inlineStr">
         <is>
           <t>2S SIN ANDRÉ LUÍZ</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="inlineStr">
+      <c r="A10" s="58" t="inlineStr">
         <is>
           <t>2S SAD TATIANNE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="inlineStr">
+      <c r="A11" s="58" t="inlineStr">
         <is>
           <t>2S SIN TADEU</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="inlineStr">
+      <c r="A12" s="58" t="inlineStr">
         <is>
           <t>2S SEL DIMAS</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="49" t="inlineStr">
+      <c r="A13" s="58" t="inlineStr">
         <is>
           <t>2S SAD CALIXTO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="inlineStr">
+      <c r="A14" s="58" t="inlineStr">
         <is>
           <t>2S SIN RODRIGUES</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="49" t="inlineStr">
+      <c r="A15" s="58" t="inlineStr">
         <is>
           <t>2S SIN ÉDER</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="inlineStr">
+      <c r="A16" s="58" t="inlineStr">
         <is>
           <t>2S SAD LEITE</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="49" t="inlineStr">
+      <c r="A17" s="58" t="inlineStr">
         <is>
           <t>2S BET CLÓVIS</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="49" t="inlineStr">
+      <c r="A18" s="58" t="inlineStr">
         <is>
           <t>2S SIN ADRIANO</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="49" t="inlineStr">
+      <c r="A19" s="58" t="inlineStr">
         <is>
           <t>2S SAD DANIELA FURTADO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="49" t="inlineStr">
+      <c r="A20" s="58" t="inlineStr">
         <is>
           <t>2S SIN ALAN</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="49" t="inlineStr">
+      <c r="A21" s="58" t="inlineStr">
         <is>
           <t>2S SIN MIRANDA</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="49" t="inlineStr">
+      <c r="A22" s="58" t="inlineStr">
         <is>
           <t>2S BET ALMEIDA</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="49" t="inlineStr">
+      <c r="A23" s="58" t="inlineStr">
         <is>
           <t>2S SAD JULIA</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="49" t="inlineStr">
+      <c r="A24" s="58" t="inlineStr">
         <is>
           <t>3S SIN SANTOS</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="49" t="inlineStr">
+      <c r="A25" s="58" t="inlineStr">
         <is>
           <t>3S SIN MOTTA</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="inlineStr">
+      <c r="A26" s="58" t="inlineStr">
         <is>
           <t>3S SIN PEDROSO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="inlineStr">
+      <c r="A27" s="58" t="inlineStr">
         <is>
           <t>3S SIN FERRAZ</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="49" t="inlineStr">
+      <c r="A28" s="58" t="inlineStr">
         <is>
           <t>3S SIN LEON</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="49" t="inlineStr">
+      <c r="A29" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve">3S SAD JONATHAS </t>
         </is>
       </c>
-      <c r="B29" s="49" t="n">
+      <c r="B29" s="58" t="n">
         <v>43765</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="49" t="inlineStr">
+      <c r="A30" s="58" t="inlineStr">
         <is>
           <t>3S SIN ALBINO</t>
         </is>
       </c>
-      <c r="B30" s="49" t="n">
+      <c r="B30" s="58" t="n">
         <v>43764</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="49" t="inlineStr">
+      <c r="A31" s="58" t="inlineStr">
         <is>
           <t>3S SIN ZÁCCARO</t>
         </is>
       </c>
-      <c r="B31" s="49" t="n">
+      <c r="B31" s="58" t="n">
         <v>43758</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="inlineStr">
+      <c r="A32" s="58" t="inlineStr">
         <is>
           <t>3S SIN SOARES</t>
         </is>
       </c>
-      <c r="B32" s="49" t="n">
+      <c r="B32" s="58" t="n">
         <v>43751</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="inlineStr">
+      <c r="A33" s="58" t="inlineStr">
         <is>
           <t>3S SIN JANUÁRIO</t>
         </is>
       </c>
-      <c r="B33" s="49" t="n">
+      <c r="B33" s="58" t="n">
         <v>43744</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="inlineStr">
+      <c r="A34" s="58" t="inlineStr">
         <is>
           <t>3S SIN VAZ</t>
         </is>
       </c>
-      <c r="B34" s="49" t="n">
+      <c r="B34" s="58" t="n">
         <v>43757</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="inlineStr">
+      <c r="A35" s="58" t="inlineStr">
         <is>
           <t>3S SIN PERROTE</t>
         </is>
       </c>
-      <c r="B35" s="49" t="n">
+      <c r="B35" s="58" t="n">
         <v>43743</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="49" t="inlineStr">
+      <c r="A36" s="58" t="inlineStr">
         <is>
           <t>3S SIN CAMPOS</t>
         </is>
       </c>
-      <c r="B36" s="49" t="n">
+      <c r="B36" s="58" t="n">
         <v>43750</v>
       </c>
     </row>
@@ -2462,7 +2465,7 @@
       <selection activeCell="D2" sqref="B2:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="24.5703125"/>
     <col customWidth="1" max="29" min="2" style="1" width="10.7109375"/>
@@ -2483,304 +2486,304 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="inlineStr">
+      <c r="A2" s="58" t="inlineStr">
         <is>
           <t>1S SGS ANDERSON</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="inlineStr">
+      <c r="A3" s="58" t="inlineStr">
         <is>
           <t>1S SAD CLAUDINO</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="inlineStr">
+      <c r="A4" s="58" t="inlineStr">
         <is>
           <t>2S SIN DAVID</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="inlineStr">
+      <c r="A5" s="58" t="inlineStr">
         <is>
           <t>2S SIN VICTOR</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="inlineStr">
+      <c r="A6" s="58" t="inlineStr">
         <is>
           <t>2S SIN SUELEN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="inlineStr">
+      <c r="A7" s="58" t="inlineStr">
         <is>
           <t>2S SCF GISELI</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="inlineStr">
+      <c r="A8" s="58" t="inlineStr">
         <is>
           <t>2S SIN BRUNO</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="inlineStr">
+      <c r="A9" s="58" t="inlineStr">
         <is>
           <t>2S SIN ANDRÉ LUÍZ</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="inlineStr">
+      <c r="A10" s="58" t="inlineStr">
         <is>
           <t>2S SAD TATIANNE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="inlineStr">
+      <c r="A11" s="58" t="inlineStr">
         <is>
           <t>2S SIN TADEU</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="inlineStr">
+      <c r="A12" s="58" t="inlineStr">
         <is>
           <t>2S SEL DIMAS</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="49" t="inlineStr">
+      <c r="A13" s="58" t="inlineStr">
         <is>
           <t>2S SAD CALIXTO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="inlineStr">
+      <c r="A14" s="58" t="inlineStr">
         <is>
           <t>2S SIN RODRIGUES</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="49" t="inlineStr">
+      <c r="A15" s="58" t="inlineStr">
         <is>
           <t>2S SIN ÉDER</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="inlineStr">
+      <c r="A16" s="58" t="inlineStr">
         <is>
           <t>2S SAD LEITE</t>
         </is>
       </c>
-      <c r="B16" s="49" t="n">
+      <c r="B16" s="58" t="n">
         <v>43769</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="49" t="inlineStr">
+      <c r="A17" s="58" t="inlineStr">
         <is>
           <t>2S BET CLÓVIS</t>
         </is>
       </c>
-      <c r="B17" s="49" t="n">
+      <c r="B17" s="58" t="n">
         <v>43768</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="49" t="inlineStr">
+      <c r="A18" s="58" t="inlineStr">
         <is>
           <t>2S SIN ADRIANO</t>
         </is>
       </c>
-      <c r="B18" s="49" t="n">
+      <c r="B18" s="58" t="n">
         <v>43767</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="49" t="inlineStr">
+      <c r="A19" s="58" t="inlineStr">
         <is>
           <t>2S SAD DANIELA FURTADO</t>
         </is>
       </c>
-      <c r="B19" s="49" t="n">
+      <c r="B19" s="58" t="n">
         <v>43766</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="49" t="inlineStr">
+      <c r="A20" s="58" t="inlineStr">
         <is>
           <t>2S SIN ALAN</t>
         </is>
       </c>
-      <c r="B20" s="49" t="n">
+      <c r="B20" s="58" t="n">
         <v>43762</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="49" t="inlineStr">
+      <c r="A21" s="58" t="inlineStr">
         <is>
           <t>2S SIN MIRANDA</t>
         </is>
       </c>
-      <c r="B21" s="49" t="n">
+      <c r="B21" s="58" t="n">
         <v>43761</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="49" t="inlineStr">
+      <c r="A22" s="58" t="inlineStr">
         <is>
           <t>2S BET ALMEIDA</t>
         </is>
       </c>
-      <c r="B22" s="49" t="n">
+      <c r="B22" s="58" t="n">
         <v>43760</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="49" t="inlineStr">
+      <c r="A23" s="58" t="inlineStr">
         <is>
           <t>2S SAD JULIA</t>
         </is>
       </c>
-      <c r="B23" s="49" t="n">
+      <c r="B23" s="58" t="n">
         <v>43759</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="49" t="inlineStr">
+      <c r="A24" s="58" t="inlineStr">
         <is>
           <t>3S SIN SANTOS</t>
         </is>
       </c>
-      <c r="B24" s="49" t="n">
+      <c r="B24" s="58" t="n">
         <v>43755</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="49" t="inlineStr">
+      <c r="A25" s="58" t="inlineStr">
         <is>
           <t>3S SIN MOTTA</t>
         </is>
       </c>
-      <c r="B25" s="49" t="n">
+      <c r="B25" s="58" t="n">
         <v>43754</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="inlineStr">
+      <c r="A26" s="58" t="inlineStr">
         <is>
           <t>* 3S SIN PEDROSO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="inlineStr">
+      <c r="A27" s="58" t="inlineStr">
         <is>
           <t>3S SIN FERRAZ</t>
         </is>
       </c>
-      <c r="B27" s="49" t="n">
+      <c r="B27" s="58" t="n">
         <v>43753</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="49" t="inlineStr">
+      <c r="A28" s="58" t="inlineStr">
         <is>
           <t>3S SIN LEON</t>
         </is>
       </c>
-      <c r="B28" s="49" t="n">
+      <c r="B28" s="58" t="n">
         <v>43752</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="49" t="inlineStr">
+      <c r="A29" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve">3S SAD JONATHAS </t>
         </is>
       </c>
-      <c r="B29" s="49" t="n">
+      <c r="B29" s="58" t="n">
         <v>43748</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="49" t="inlineStr">
+      <c r="A30" s="58" t="inlineStr">
         <is>
           <t>3S SIN ALBINO</t>
         </is>
       </c>
-      <c r="B30" s="49" t="n">
+      <c r="B30" s="58" t="n">
         <v>43747</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="49" t="inlineStr">
+      <c r="A31" s="58" t="inlineStr">
         <is>
           <t>3S SIN ZÁCCARO</t>
         </is>
       </c>
-      <c r="B31" s="49" t="n">
+      <c r="B31" s="58" t="n">
         <v>43746</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="inlineStr">
+      <c r="A32" s="58" t="inlineStr">
         <is>
           <t>3S SIN SOARES</t>
         </is>
       </c>
-      <c r="B32" s="49" t="n">
+      <c r="B32" s="58" t="n">
         <v>43745</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="inlineStr">
+      <c r="A33" s="58" t="inlineStr">
         <is>
           <t>3S SIN JANUÁRIO</t>
         </is>
       </c>
-      <c r="B33" s="49" t="n">
+      <c r="B33" s="58" t="n">
         <v>43741</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="inlineStr">
+      <c r="A34" s="58" t="inlineStr">
         <is>
           <t>* 3S SIN VAZ</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="inlineStr">
+      <c r="A35" s="58" t="inlineStr">
         <is>
           <t>3S SIN PERROTE</t>
         </is>
       </c>
-      <c r="B35" s="49" t="n">
+      <c r="B35" s="58" t="n">
         <v>43740</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="49" t="inlineStr">
+      <c r="A36" s="58" t="inlineStr">
         <is>
           <t>3S SIN CAMPOS</t>
         </is>
       </c>
-      <c r="B36" s="49" t="n">
+      <c r="B36" s="58" t="n">
         <v>43739</v>
       </c>
     </row>
@@ -2801,7 +2804,7 @@
       <selection activeCell="C15" sqref="B15:C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="24.5703125"/>
     <col customWidth="1" max="29" min="2" style="1" width="10.7109375"/>
@@ -2822,259 +2825,259 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="inlineStr">
+      <c r="A2" s="58" t="inlineStr">
         <is>
           <t>1S SGS ANDERSON</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="inlineStr">
+      <c r="A3" s="58" t="inlineStr">
         <is>
           <t>1S SAD CLAUDINO</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="inlineStr">
+      <c r="A4" s="58" t="inlineStr">
         <is>
           <t>2S SIN DAVID</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="inlineStr">
+      <c r="A5" s="58" t="inlineStr">
         <is>
           <t>2S SIN VICTOR</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="inlineStr">
+      <c r="A6" s="58" t="inlineStr">
         <is>
           <t>2S SIN SUELEN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="inlineStr">
+      <c r="A7" s="58" t="inlineStr">
         <is>
           <t>2S SCF GISELI</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="inlineStr">
+      <c r="A8" s="58" t="inlineStr">
         <is>
           <t>2S SIN BRUNO</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="inlineStr">
+      <c r="A9" s="58" t="inlineStr">
         <is>
           <t>2S SIN ANDRÉ LUÍZ</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="inlineStr">
+      <c r="A10" s="58" t="inlineStr">
         <is>
           <t>2S SAD TATIANNE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="inlineStr">
+      <c r="A11" s="58" t="inlineStr">
         <is>
           <t>2S SIN TADEU</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="inlineStr">
+      <c r="A12" s="58" t="inlineStr">
         <is>
           <t>2S SEL DIMAS</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="49" t="inlineStr">
+      <c r="A13" s="58" t="inlineStr">
         <is>
           <t>2S SAD CALIXTO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="inlineStr">
+      <c r="A14" s="58" t="inlineStr">
         <is>
           <t>2S SIN RODRIGUES</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="49" t="inlineStr">
+      <c r="A15" s="58" t="inlineStr">
         <is>
           <t>2S SIN ÉDER</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="inlineStr">
+      <c r="A16" s="58" t="inlineStr">
         <is>
           <t>2S SAD LEITE</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="49" t="inlineStr">
+      <c r="A17" s="58" t="inlineStr">
         <is>
           <t>2S BET CLÓVIS</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="49" t="inlineStr">
+      <c r="A18" s="58" t="inlineStr">
         <is>
           <t>2S SIN ADRIANO</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="49" t="inlineStr">
+      <c r="A19" s="58" t="inlineStr">
         <is>
           <t>2S SAD DANIELA FURTADO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="49" t="inlineStr">
+      <c r="A20" s="58" t="inlineStr">
         <is>
           <t>2S SIN ALAN</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="49" t="inlineStr">
+      <c r="A21" s="58" t="inlineStr">
         <is>
           <t>2S SIN MIRANDA</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="49" t="inlineStr">
+      <c r="A22" s="58" t="inlineStr">
         <is>
           <t>2S BET ALMEIDA</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="49" t="inlineStr">
+      <c r="A23" s="58" t="inlineStr">
         <is>
           <t>2S SAD JULIA</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="49" t="inlineStr">
+      <c r="A24" s="58" t="inlineStr">
         <is>
           <t>3S SIN SANTOS</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="49" t="inlineStr">
+      <c r="A25" s="58" t="inlineStr">
         <is>
           <t>3S SIN MOTTA</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="inlineStr">
+      <c r="A26" s="58" t="inlineStr">
         <is>
           <t>* 3S SIN PEDROSO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="inlineStr">
+      <c r="A27" s="58" t="inlineStr">
         <is>
           <t>3S SIN FERRAZ</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="49" t="inlineStr">
+      <c r="A28" s="58" t="inlineStr">
         <is>
           <t>3S SIN LEON</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="49" t="inlineStr">
+      <c r="A29" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve">3S SAD JONATHAS </t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="49" t="inlineStr">
+      <c r="A30" s="58" t="inlineStr">
         <is>
           <t>3S SIN ALBINO</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="49" t="inlineStr">
+      <c r="A31" s="58" t="inlineStr">
         <is>
           <t>3S SIN ZÁCCARO</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="inlineStr">
+      <c r="A32" s="58" t="inlineStr">
         <is>
           <t>3S SIN SOARES</t>
         </is>
       </c>
-      <c r="B32" s="49" t="n">
+      <c r="B32" s="58" t="n">
         <v>43763</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="inlineStr">
+      <c r="A33" s="58" t="inlineStr">
         <is>
           <t>3S SIN JANUÁRIO</t>
         </is>
       </c>
-      <c r="B33" s="49" t="n">
+      <c r="B33" s="58" t="n">
         <v>43756</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="inlineStr">
+      <c r="A34" s="58" t="inlineStr">
         <is>
           <t>* 3S SIN VAZ</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="inlineStr">
+      <c r="A35" s="58" t="inlineStr">
         <is>
           <t>3S SIN PERROTE</t>
         </is>
       </c>
-      <c r="B35" s="49" t="n">
+      <c r="B35" s="58" t="n">
         <v>43749</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="49" t="inlineStr">
+      <c r="A36" s="58" t="inlineStr">
         <is>
           <t>3S SIN CAMPOS</t>
         </is>
       </c>
-      <c r="B36" s="49" t="n">
+      <c r="B36" s="58" t="n">
         <v>43742</v>
       </c>
     </row>
@@ -3096,7 +3099,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.7109375" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="19" width="24.5703125"/>
     <col customWidth="1" max="29" min="2" style="1" width="10.7109375"/>
@@ -3140,271 +3143,271 @@
       <c r="AC1" s="21" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="inlineStr">
+      <c r="A2" s="58" t="inlineStr">
         <is>
           <t>1S SGS ANDERSON</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="inlineStr">
+      <c r="A3" s="58" t="inlineStr">
         <is>
           <t>1S SAD CLAUDINO</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="inlineStr">
+      <c r="A4" s="58" t="inlineStr">
         <is>
           <t>2S SIN DAVID</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="inlineStr">
+      <c r="A5" s="58" t="inlineStr">
         <is>
           <t>2S SIN VICTOR</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="inlineStr">
+      <c r="A6" s="58" t="inlineStr">
         <is>
           <t>2S SIN SUELEN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="inlineStr">
+      <c r="A7" s="58" t="inlineStr">
         <is>
           <t>2S SCF GISELI</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="inlineStr">
+      <c r="A8" s="58" t="inlineStr">
         <is>
           <t>2S SIN BRUNO</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="inlineStr">
+      <c r="A9" s="58" t="inlineStr">
         <is>
           <t>2S SIN ANDRÉ LUÍZ</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="inlineStr">
+      <c r="A10" s="58" t="inlineStr">
         <is>
           <t>2S SAD TATIANNE</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="inlineStr">
+      <c r="A11" s="58" t="inlineStr">
         <is>
           <t>2S SIN TADEU</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="inlineStr">
+      <c r="A12" s="58" t="inlineStr">
         <is>
           <t>2S SEL DIMAS</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="49" t="inlineStr">
+      <c r="A13" s="58" t="inlineStr">
         <is>
           <t>2S SAD CALIXTO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="inlineStr">
+      <c r="A14" s="58" t="inlineStr">
         <is>
           <t>2S SIN RODRIGUES</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="49" t="inlineStr">
+      <c r="A15" s="58" t="inlineStr">
         <is>
           <t>2S SIN ÉDER</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="inlineStr">
+      <c r="A16" s="58" t="inlineStr">
         <is>
           <t>2S SAD LEITE</t>
         </is>
       </c>
-      <c r="B16" s="49" t="inlineStr">
+      <c r="B16" s="58" t="inlineStr">
         <is>
           <t>Lastro</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="49" t="inlineStr">
+      <c r="A17" s="58" t="inlineStr">
         <is>
           <t>2S BET CLÓVIS</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="49" t="inlineStr">
+      <c r="A18" s="58" t="inlineStr">
         <is>
           <t>2S SIN ADRIANO</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="49" t="inlineStr">
+      <c r="A19" s="58" t="inlineStr">
         <is>
           <t>2S SAD DANIELA FURTADO</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="49" t="inlineStr">
+      <c r="A20" s="58" t="inlineStr">
         <is>
           <t>2S SIN ALAN</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="49" t="inlineStr">
+      <c r="A21" s="58" t="inlineStr">
         <is>
           <t>2S SIN MIRANDA</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="49" t="inlineStr">
+      <c r="A22" s="58" t="inlineStr">
         <is>
           <t>2S BET ALMEIDA</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="49" t="inlineStr">
+      <c r="A23" s="58" t="inlineStr">
         <is>
           <t>2S SAD JULIA</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="49" t="inlineStr">
+      <c r="A24" s="58" t="inlineStr">
         <is>
           <t>3S SIN SANTOS</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="49" t="inlineStr">
+      <c r="A25" s="58" t="inlineStr">
         <is>
           <t>3S SIN MOTTA</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="inlineStr">
+      <c r="A26" s="58" t="inlineStr">
         <is>
           <t>3S SIN PEDROSO</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="inlineStr">
+      <c r="A27" s="58" t="inlineStr">
         <is>
           <t>3S SIN FERRAZ</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="49" t="inlineStr">
+      <c r="A28" s="58" t="inlineStr">
         <is>
           <t>3S SIN LEON</t>
         </is>
       </c>
-      <c r="B28" s="49" t="n">
+      <c r="B28" s="58" t="n">
         <v>43824</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="49" t="inlineStr">
+      <c r="A29" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve">3S SAD JONATHAS </t>
         </is>
       </c>
-      <c r="B29" s="49" t="n">
+      <c r="B29" s="58" t="n">
         <v>43823</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="49" t="inlineStr">
+      <c r="A30" s="58" t="inlineStr">
         <is>
           <t>3S SIN ALBINO</t>
         </is>
       </c>
-      <c r="B30" s="49" t="n">
+      <c r="B30" s="58" t="n">
         <v>43702</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="49" t="inlineStr">
+      <c r="A31" s="58" t="inlineStr">
         <is>
           <t>3S SIN ZÁCCARO</t>
         </is>
       </c>
-      <c r="B31" s="49" t="n">
+      <c r="B31" s="58" t="n">
         <v>43701</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="inlineStr">
+      <c r="A32" s="58" t="inlineStr">
         <is>
           <t>3S SIN SOARES</t>
         </is>
       </c>
-      <c r="B32" s="49" t="n">
+      <c r="B32" s="58" t="n">
         <v>43641</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="inlineStr">
+      <c r="A33" s="58" t="inlineStr">
         <is>
           <t>3S SIN JANUÁRIO</t>
         </is>
       </c>
-      <c r="B33" s="49" t="n">
+      <c r="B33" s="58" t="n">
         <v>43703</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="inlineStr">
+      <c r="A34" s="58" t="inlineStr">
         <is>
           <t>3S SIN VAZ</t>
         </is>
       </c>
-      <c r="B34" s="49" t="n">
+      <c r="B34" s="58" t="n">
         <v>43642</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="inlineStr">
+      <c r="A35" s="58" t="inlineStr">
         <is>
           <t>3S SIN PERROTE</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="49" t="inlineStr">
+      <c r="A36" s="58" t="inlineStr">
         <is>
           <t>3S SIN CAMPOS</t>
         </is>
@@ -3427,7 +3430,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="47" width="14"/>
     <col customWidth="1" max="2" min="2" style="47" width="26"/>
@@ -4170,7 +4173,7 @@
       </c>
       <c r="B44" s="53" t="inlineStr">
         <is>
-          <t>2S SAD JULIA</t>
+          <t>2S SIN MIRANDA</t>
         </is>
       </c>
       <c r="C44" s="54" t="inlineStr"/>
@@ -4184,7 +4187,7 @@
       </c>
       <c r="B45" s="53" t="inlineStr">
         <is>
-          <t>2S SIN MIRANDA</t>
+          <t>2S SAD JULIA</t>
         </is>
       </c>
       <c r="C45" s="54" t="inlineStr"/>

</xml_diff>